<commit_message>
feat: add more code for strain design
</commit_message>
<xml_diff>
--- a/result/fseof_df_result_for_Kmarx.xlsx
+++ b/result/fseof_df_result_for_Kmarx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xluhon/Documents/GitHub/Yli_GEMs/result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43962313-3A9D-4A4C-85C9-669EC82822CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E9BEBF-A9CD-D84D-A546-091842238BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="15220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38800" yWindow="500" windowWidth="27880" windowHeight="21440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -647,7 +647,7 @@
   <dimension ref="A1:M85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>